<commit_message>
Adding Firefox Driver to the project and update test data
</commit_message>
<xml_diff>
--- a/Selenium with CSharp/Selenium with CSharp/DataDriven/Data1.xlsx
+++ b/Selenium with CSharp/Selenium with CSharp/DataDriven/Data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed.Mohamed\Documents\GitHub\Selenium-c-\Selenium with CSharp\Selenium with CSharp\DataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE46F2F-85FD-47D1-815C-67B7E672BC35}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F14302-B6F7-4927-869A-68492AD66E6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
   </bookViews>
@@ -72,16 +72,16 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>TestAuto_POC18sep</t>
-  </si>
-  <si>
-    <t>Facility_POC18sep</t>
-  </si>
-  <si>
-    <t>Pharmacy_POC18sep</t>
-  </si>
-  <si>
-    <t>AlignmentProjectPOC18sep</t>
+    <t>TestAuto_POC30sep</t>
+  </si>
+  <si>
+    <t>Facility_POC30sep</t>
+  </si>
+  <si>
+    <t>Pharmacy_POC30sep</t>
+  </si>
+  <si>
+    <t>AlignmentProjectPOC30sep</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Adding validation class in data base and modify test data and update some steps in the script related to Alignment Project Class
</commit_message>
<xml_diff>
--- a/Selenium with CSharp/Selenium with CSharp/DataDriven/Data1.xlsx
+++ b/Selenium with CSharp/Selenium with CSharp/DataDriven/Data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed.Mohamed\Documents\GitHub\Selenium-c-\Selenium with CSharp\Selenium with CSharp\DataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F14302-B6F7-4927-869A-68492AD66E6F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBB2331-14C1-4FB2-AA0E-2D948123CB17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
   </bookViews>
@@ -54,12 +54,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>maha.moustafa@bd.com</t>
-  </si>
-  <si>
-    <t>Carefusion@4</t>
-  </si>
-  <si>
     <t>IDN Name</t>
   </si>
   <si>
@@ -72,16 +66,22 @@
     <t>Cerner</t>
   </si>
   <si>
-    <t>TestAuto_POC30sep</t>
-  </si>
-  <si>
-    <t>Facility_POC30sep</t>
-  </si>
-  <si>
-    <t>Pharmacy_POC30sep</t>
-  </si>
-  <si>
-    <t>AlignmentProjectPOC30sep</t>
+    <t>Rola.khalaf2@bd.com</t>
+  </si>
+  <si>
+    <t>Carefusion@5</t>
+  </si>
+  <si>
+    <t>TestAuto_POC31sep</t>
+  </si>
+  <si>
+    <t>Facility_POC31sep</t>
+  </si>
+  <si>
+    <t>Pharmacy_POC31sep</t>
+  </si>
+  <si>
+    <t>Epic1011024</t>
   </si>
 </sst>
 </file>
@@ -649,7 +649,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +667,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -675,7 +675,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -690,10 +690,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
@@ -708,7 +708,7 @@
         <v>4</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>0</v>
@@ -734,7 +734,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H5" s="18" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
1- Update Test data file 2- Organize the project scipt
</commit_message>
<xml_diff>
--- a/Selenium with CSharp/Selenium with CSharp/DataDriven/Data1.xlsx
+++ b/Selenium with CSharp/Selenium with CSharp/DataDriven/Data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed.Mohamed\Documents\GitHub\Selenium-c-\Selenium with CSharp\Selenium with CSharp\DataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBB2331-14C1-4FB2-AA0E-2D948123CB17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2867B1D6-CCA2-40CC-BD85-5691CB8981A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
   </bookViews>
@@ -72,16 +72,16 @@
     <t>Carefusion@5</t>
   </si>
   <si>
-    <t>TestAuto_POC31sep</t>
-  </si>
-  <si>
-    <t>Facility_POC31sep</t>
-  </si>
-  <si>
-    <t>Pharmacy_POC31sep</t>
-  </si>
-  <si>
-    <t>Epic1011024</t>
+    <t>Project222</t>
+  </si>
+  <si>
+    <t>POC5OCTo</t>
+  </si>
+  <si>
+    <t>FacilityPOC5OCTo</t>
+  </si>
+  <si>
+    <t>PharmacyPOC5OCTo</t>
   </si>
 </sst>
 </file>
@@ -649,7 +649,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,28 +716,28 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -746,5 +746,6 @@
     <hyperlink ref="B2" r:id="rId2" xr:uid="{2CE672E2-3C1C-4455-A9C8-06DEDBEEF801}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
1. Adding Capturing screenshots at the end of each test 2. Update the validation class [adding screenshots names] 3. Update test data excel file
</commit_message>
<xml_diff>
--- a/Selenium with CSharp/Selenium with CSharp/DataDriven/Data1.xlsx
+++ b/Selenium with CSharp/Selenium with CSharp/DataDriven/Data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed.Mohamed\Documents\GitHub\Selenium-c-\Selenium with CSharp\Selenium with CSharp\DataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2867B1D6-CCA2-40CC-BD85-5691CB8981A7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542B5D66-753B-48B4-AD36-13AB61C03615}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
   </bookViews>
@@ -75,13 +75,13 @@
     <t>Project222</t>
   </si>
   <si>
-    <t>POC5OCTo</t>
-  </si>
-  <si>
-    <t>FacilityPOC5OCTo</t>
-  </si>
-  <si>
-    <t>PharmacyPOC5OCTo</t>
+    <t>POC15OCTo</t>
+  </si>
+  <si>
+    <t>FacilityPOC15OCTo</t>
+  </si>
+  <si>
+    <t>PharmacyPOC15OCTo</t>
   </si>
 </sst>
 </file>
@@ -649,7 +649,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update Test Data Modify The script due to the changes occured on Stage A server
</commit_message>
<xml_diff>
--- a/Selenium with CSharp/Selenium with CSharp/DataDriven/Data1.xlsx
+++ b/Selenium with CSharp/Selenium with CSharp/DataDriven/Data1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ahmed.Mohamed\Documents\GitHub\Selenium-c-\Selenium with CSharp\Selenium with CSharp\DataDriven\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542B5D66-753B-48B4-AD36-13AB61C03615}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0409F6C2-ACD7-4CC1-AB4D-747D7EADE9EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CA5A8F89-FF04-4289-9E9B-FF6BE77DC74E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Alignment Project Name</t>
   </si>
@@ -75,13 +75,13 @@
     <t>Project222</t>
   </si>
   <si>
-    <t>POC15OCTo</t>
-  </si>
-  <si>
-    <t>FacilityPOC15OCTo</t>
-  </si>
-  <si>
-    <t>PharmacyPOC15OCTo</t>
+    <t>AH_healthsys_poc1</t>
+  </si>
+  <si>
+    <t>Facility_POC_2</t>
+  </si>
+  <si>
+    <t>Pharmacy_POC_2</t>
   </si>
 </sst>
 </file>
@@ -648,21 +648,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05CF6C07-F7D2-4879-98C8-38A47B6B27B6}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="4" width="29.28515625" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" customWidth="1"/>
-    <col min="6" max="7" width="21" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.5546875" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" customWidth="1"/>
+    <col min="3" max="4" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" customWidth="1"/>
+    <col min="6" max="6" width="26.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>5</v>
       </c>
@@ -670,7 +671,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -678,7 +679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11"/>
       <c r="B3" s="14"/>
       <c r="C3" s="12"/>
@@ -688,7 +689,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
@@ -714,7 +715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="17" t="s">
         <v>14</v>
       </c>
@@ -724,8 +725,8 @@
       <c r="C5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>15</v>
+      <c r="D5" s="8">
+        <v>4112019</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>16</v>

</xml_diff>